<commit_message>
Update old Elaun Hotel atau Lojing Gred SSPA (Dalam Negeri) - Copy.xlsx
</commit_message>
<xml_diff>
--- a/7 Dalam Negeri/old Elaun Hotel atau Lojing Gred SSPA (Dalam Negeri) - Copy.xlsx
+++ b/7 Dalam Negeri/old Elaun Hotel atau Lojing Gred SSPA (Dalam Negeri) - Copy.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -1244,7 +1244,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>

</xml_diff>